<commit_message>
Reunion del 8 de octubre
</commit_message>
<xml_diff>
--- a/Seguimiento/Task Board.xlsx
+++ b/Seguimiento/Task Board.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Moderadores" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Backlog</t>
   </si>
@@ -33,9 +33,6 @@
     <t>RF. 008 Registrar pago</t>
   </si>
   <si>
-    <t>Sprint BackLog</t>
-  </si>
-  <si>
     <t>Para Hacer</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>RF. 004 ABM Empleado</t>
   </si>
   <si>
-    <t>RF. 012 Setup Proyecto</t>
-  </si>
-  <si>
     <t>RF. 011 Registrar Stock (WS)</t>
   </si>
   <si>
@@ -127,6 +121,72 @@
   </si>
   <si>
     <t>Complejidades</t>
+  </si>
+  <si>
+    <t>Esto pertenece al sistema de facturación</t>
+  </si>
+  <si>
+    <t>Pertenece al sist. De stock</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Calificar cuando se especifique</t>
+  </si>
+  <si>
+    <t>Pedir y reponer stock</t>
+  </si>
+  <si>
+    <t>RF. 012.1 Setup Proyecto BBDD</t>
+  </si>
+  <si>
+    <t>RF. 012.2 Setup Proyecto Aplicación</t>
+  </si>
+  <si>
+    <t>RF.013 Automatización de Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linux </t>
+  </si>
+  <si>
+    <t>Postgres</t>
+  </si>
+  <si>
+    <t>Ruby</t>
+  </si>
+  <si>
+    <t>Rails</t>
+  </si>
+  <si>
+    <t>Selenium \ Otro</t>
+  </si>
+  <si>
+    <t>UML \ Diagramas</t>
+  </si>
+  <si>
+    <t>Jquery \ Javascript</t>
+  </si>
+  <si>
+    <t>Github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herramientas de reporte </t>
+  </si>
+  <si>
+    <t>Sprint 0</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Uml \ Diagramas</t>
+  </si>
+  <si>
+    <t>Setup Proyecto BBDD</t>
+  </si>
+  <si>
+    <t>Linux</t>
   </si>
 </sst>
 </file>
@@ -180,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -328,22 +388,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -359,6 +408,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,14 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -670,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:L15"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -681,7 +735,7 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -690,163 +744,323 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:12" ht="15.75" thickBot="1">
-      <c r="H2" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="H2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="L3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="18"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="19">
+        <v>30</v>
+      </c>
+      <c r="D4" s="16">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="20"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="18">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="21">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="20"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="22">
+        <v>23</v>
+      </c>
+      <c r="D6" s="19">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B7" s="17"/>
+      <c r="C7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="18">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
         <v>15</v>
       </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="20"/>
-      <c r="C7" s="13" t="s">
+    </row>
+    <row r="8" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B8" s="17"/>
+      <c r="C8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D8" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12">
+      <c r="B9" s="17"/>
+      <c r="C9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="18">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12">
-      <c r="B8" s="20"/>
-      <c r="C8" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
-      <c r="B9" s="20"/>
-      <c r="C9" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="21">
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12">
+      <c r="B10" s="17"/>
+      <c r="C10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="2:12">
-      <c r="B10" s="20"/>
-      <c r="C10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="21"/>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="20"/>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="21"/>
+      <c r="D11" s="18"/>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="20"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="20"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="D13" s="18">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="20"/>
+      <c r="B14" s="17">
+        <v>11</v>
+      </c>
       <c r="C14" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="21"/>
-    </row>
-    <row r="15" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B15" s="23"/>
-      <c r="C15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="D14" s="18">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12">
+      <c r="B15" s="17">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12">
+      <c r="B16" s="17">
+        <v>5</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="26"/>
+      <c r="B17" s="17">
+        <v>9</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="28">
+        <v>20</v>
+      </c>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" s="17">
+        <v>3</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" s="17">
+        <v>4</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="17">
+        <v>6</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="17">
+        <v>7</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="17">
+        <v>10</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="17"/>
+      <c r="C23" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="17">
+        <v>1</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="17">
+        <v>8</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="14">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="B4:C15">
@@ -864,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -877,7 +1091,7 @@
     <row r="1" spans="2:3" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:3" ht="15.75" thickBot="1">
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -886,7 +1100,7 @@
         <v>41913</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:3">
@@ -894,7 +1108,7 @@
         <v>41920</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -902,7 +1116,7 @@
         <v>41927</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -910,7 +1124,7 @@
         <v>41934</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -918,7 +1132,7 @@
         <v>41941</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:3">
@@ -926,7 +1140,7 @@
         <v>41948</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:3">

</xml_diff>